<commit_message>
replaced albany d file
</commit_message>
<xml_diff>
--- a/raw/20000822/AL-D-2000.xlsx
+++ b/raw/20000822/AL-D-2000.xlsx
@@ -2,16 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
-  <workbookPr autoCompressPictures="0"/>
+  <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17640" windowHeight="9080" tabRatio="201"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15960" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="A" sheetId="1" r:id="rId1"/>
-    <sheet name="B" sheetId="2" r:id="rId2"/>
-    <sheet name="C" sheetId="3" r:id="rId3"/>
+    <sheet name="20000822__wy__democratic__prima" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -488,14 +486,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
-    <tabColor rgb="FFFFFFFF"/>
-  </sheetPr>
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:15">
       <c r="B1" t="s">
@@ -997,100 +992,38 @@
         <v>32</v>
       </c>
       <c r="B21">
-        <f>SUM(B6:B19)</f>
         <v>1884</v>
       </c>
       <c r="C21">
-        <f>SUM(C6:C19)</f>
         <v>918</v>
       </c>
       <c r="D21">
-        <f>SUM(D6:D19)</f>
         <v>490</v>
       </c>
       <c r="F21">
-        <f>SUM(F6:F19)</f>
         <v>874</v>
       </c>
       <c r="G21">
-        <f>SUM(G6:G19)</f>
         <v>609</v>
       </c>
       <c r="I21">
-        <f>SUM(I6:I19)</f>
         <v>367</v>
       </c>
       <c r="J21" t="s">
         <v>32</v>
       </c>
       <c r="K21">
-        <f>SUM(K6:K19)</f>
         <v>319</v>
       </c>
       <c r="M21">
-        <f>SUM(M6:M19)</f>
         <v>410</v>
       </c>
       <c r="O21">
-        <f>SUM(O6:O19)</f>
         <v>546</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
-    <tabColor rgb="FFFFFFFF"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
-    <tabColor rgb="FFFFFFFF"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>